<commit_message>
validation 3C, oublié d'enregitrer.....
</commit_message>
<xml_diff>
--- a/P5_02_plantests.xlsx
+++ b/P5_02_plantests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1b5709471efc6e4/Desktop/Ocarino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53822717-0740-4C70-A759-034BE82C7631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{53822717-0740-4C70-A759-034BE82C7631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89F4D8CD-F206-4D28-BF84-B10CF865BFC0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{33E599D9-9426-4C6A-88A2-96C8F0BE5623}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Script_accueil.js</t>
   </si>
   <si>
-    <t>23-90</t>
-  </si>
-  <si>
     <t>createCard</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>getIdFromUrl</t>
   </si>
   <si>
-    <t>19-24</t>
-  </si>
-  <si>
     <t>La fonction reçoit en paramètre les données de l'API via un fetch.  Puis elle crée l'architecture HTML et génère le contenu dynamiquement. Elle crée également un bouton qui renvoit vers la page produit.html. L'id du produit est intégré à l'url de produit.html</t>
   </si>
   <si>
@@ -96,9 +90,6 @@
     <t>getProductInfo</t>
   </si>
   <si>
-    <t>28-44</t>
-  </si>
-  <si>
     <t>la fonction retourne la response.json() et console.log la fonction 1</t>
   </si>
   <si>
@@ -106,9 +97,6 @@
   </si>
   <si>
     <t>La fonction appelle getIdFromUrl pour récuperer les informations liées au produit que la page doit afficher. Elle recoit en parametre l'url de l'api + l'id du produit concerné.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68 - 146 </t>
   </si>
   <si>
     <t>fonction1</t>
@@ -121,9 +109,6 @@
 Les informations ne sont pas stockées dans le local storage. </t>
   </si>
   <si>
-    <t>150 - 152</t>
-  </si>
-  <si>
     <t xml:space="preserve">Le nombre d'articles ajoutés au panier et donc au local storage doit s'afficher dans la navigation et s'incrémenter de 1 à chaque clic sur le bouton ajouter au panier. </t>
   </si>
   <si>
@@ -133,9 +118,6 @@
     <t xml:space="preserve">Le chiffre ne s'incrémente pas lors de l'ajout d'un produit issu d'une autre page. </t>
   </si>
   <si>
-    <t>21 - 71</t>
-  </si>
-  <si>
     <t>panier.js</t>
   </si>
   <si>
@@ -163,12 +145,6 @@
     <t xml:space="preserve">L'encart ne disparait pas et ce n'est pas le bon article qui est supprimé. </t>
   </si>
   <si>
-    <t>101 - 115</t>
-  </si>
-  <si>
-    <t>75 - 80</t>
-  </si>
-  <si>
     <t>panierVide</t>
   </si>
   <si>
@@ -178,9 +154,6 @@
     <t xml:space="preserve">Le texte s'affiche alors que le panier n'est pas vide. </t>
   </si>
   <si>
-    <t>81 - 88</t>
-  </si>
-  <si>
     <t>displayFormulaire</t>
   </si>
   <si>
@@ -193,9 +166,6 @@
     <t xml:space="preserve">Le formulaire reste affiché alors que le panier est vide. </t>
   </si>
   <si>
-    <t>90 - 96</t>
-  </si>
-  <si>
     <t>displayMontant</t>
   </si>
   <si>
@@ -214,9 +184,6 @@
     <t>prixTotal</t>
   </si>
   <si>
-    <t>121 - 136</t>
-  </si>
-  <si>
     <t xml:space="preserve">La fonction calcule le prix total à payer en fonction des articles au panier. </t>
   </si>
   <si>
@@ -224,12 +191,6 @@
   </si>
   <si>
     <t xml:space="preserve">La somme ne se met pas à jour. </t>
-  </si>
-  <si>
-    <t>envoieFormulaire</t>
-  </si>
-  <si>
-    <t>141 - 179</t>
   </si>
   <si>
     <t xml:space="preserve">La fonction envoie au serveur via un fetch methode POST les données du formulaire de commande au clic sur le bouton "commander". Le serveur doit renvoyer un orderId que la fonction envoieFormulaire ajouter à l'url de la page confirmation.html. Celle-ci s'ouvre également lorsque l'utilisateur clic sur le bouton commander. </t>
@@ -263,9 +224,6 @@
     <t>getPrixTotal</t>
   </si>
   <si>
-    <t>8-20</t>
-  </si>
-  <si>
     <t xml:space="preserve">La fonction récupere les données prix du local storage et en fait la somme. </t>
   </si>
   <si>
@@ -275,9 +233,6 @@
     <t>displayMessage</t>
   </si>
   <si>
-    <t>24-42</t>
-  </si>
-  <si>
     <t>La fonction affiche récupere l'orderId, le prix totale, crée la structure html de la page et affiche un message de remerciement pour la commande</t>
   </si>
   <si>
@@ -288,6 +243,51 @@
   </si>
   <si>
     <t xml:space="preserve">la fonction ne récupere pas correctement le prix et l'order Id. Le texte du message ne s'affiche pas. </t>
+  </si>
+  <si>
+    <t>17-77</t>
+  </si>
+  <si>
+    <t>16-21</t>
+  </si>
+  <si>
+    <t>25-39</t>
+  </si>
+  <si>
+    <t>59-129</t>
+  </si>
+  <si>
+    <t>133-135</t>
+  </si>
+  <si>
+    <t>16-59</t>
+  </si>
+  <si>
+    <t>89-102</t>
+  </si>
+  <si>
+    <t>63-68</t>
+  </si>
+  <si>
+    <t>70-76</t>
+  </si>
+  <si>
+    <t>78-84</t>
+  </si>
+  <si>
+    <t>105-119</t>
+  </si>
+  <si>
+    <t>123-160</t>
+  </si>
+  <si>
+    <t>envoiFormulaire</t>
+  </si>
+  <si>
+    <t>8-19</t>
+  </si>
+  <si>
+    <t>23-41</t>
   </si>
 </sst>
 </file>
@@ -672,7 +672,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -711,296 +711,296 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>